<commit_message>
aggiornato Bloomberg company ID
</commit_message>
<xml_diff>
--- a/Investment Object VBA/Bloomberg company ID.xlsx
+++ b/Investment Object VBA/Bloomberg company ID.xlsx
@@ -16,27 +16,300 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
-  <si>
-    <t>Claudio</t>
-  </si>
-  <si>
-    <t>Reto</t>
-  </si>
-  <si>
-    <t>Sandro</t>
-  </si>
-  <si>
-    <t>Carlo</t>
-  </si>
-  <si>
-    <t>Riccardo</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
   <si>
     <t>Counterparty</t>
   </si>
   <si>
-    <t>Luciana</t>
+    <t>328069</t>
+  </si>
+  <si>
+    <t>825197</t>
+  </si>
+  <si>
+    <t>115227</t>
+  </si>
+  <si>
+    <t>100012</t>
+  </si>
+  <si>
+    <t>11585426</t>
+  </si>
+  <si>
+    <t>115649</t>
+  </si>
+  <si>
+    <t>136124</t>
+  </si>
+  <si>
+    <t>101695</t>
+  </si>
+  <si>
+    <t>225547</t>
+  </si>
+  <si>
+    <t>116664</t>
+  </si>
+  <si>
+    <t>100158</t>
+  </si>
+  <si>
+    <t>101032</t>
+  </si>
+  <si>
+    <t>115682</t>
+  </si>
+  <si>
+    <t>311449</t>
+  </si>
+  <si>
+    <t>115245</t>
+  </si>
+  <si>
+    <t>196812</t>
+  </si>
+  <si>
+    <t>221358</t>
+  </si>
+  <si>
+    <t>23601414</t>
+  </si>
+  <si>
+    <t>215188</t>
+  </si>
+  <si>
+    <t>32957556</t>
+  </si>
+  <si>
+    <t>128058</t>
+  </si>
+  <si>
+    <t>115268</t>
+  </si>
+  <si>
+    <t>100285</t>
+  </si>
+  <si>
+    <t>11266676</t>
+  </si>
+  <si>
+    <t>17292024</t>
+  </si>
+  <si>
+    <t>112699</t>
+  </si>
+  <si>
+    <t>156262</t>
+  </si>
+  <si>
+    <t>20696265</t>
+  </si>
+  <si>
+    <t>115662</t>
+  </si>
+  <si>
+    <t>338683</t>
+  </si>
+  <si>
+    <t>115259</t>
+  </si>
+  <si>
+    <t>384888</t>
+  </si>
+  <si>
+    <t>304968</t>
+  </si>
+  <si>
+    <t>186881</t>
+  </si>
+  <si>
+    <t>12257737</t>
+  </si>
+  <si>
+    <t>918049</t>
+  </si>
+  <si>
+    <t>143031</t>
+  </si>
+  <si>
+    <t>181934</t>
+  </si>
+  <si>
+    <t>833413</t>
+  </si>
+  <si>
+    <t>180971</t>
+  </si>
+  <si>
+    <t>128107</t>
+  </si>
+  <si>
+    <t>180000</t>
+  </si>
+  <si>
+    <t>180969</t>
+  </si>
+  <si>
+    <t>29569991</t>
+  </si>
+  <si>
+    <t>16123514</t>
+  </si>
+  <si>
+    <t>156070</t>
+  </si>
+  <si>
+    <t>217232</t>
+  </si>
+  <si>
+    <t>100632</t>
+  </si>
+  <si>
+    <t>348768</t>
+  </si>
+  <si>
+    <t>115725</t>
+  </si>
+  <si>
+    <t>115823</t>
+  </si>
+  <si>
+    <t>128042</t>
+  </si>
+  <si>
+    <t>100312</t>
+  </si>
+  <si>
+    <t>1489029</t>
+  </si>
+  <si>
+    <t>191053</t>
+  </si>
+  <si>
+    <t>191081</t>
+  </si>
+  <si>
+    <t>180978</t>
+  </si>
+  <si>
+    <t>101173</t>
+  </si>
+  <si>
+    <t>115442</t>
+  </si>
+  <si>
+    <t>1797989</t>
+  </si>
+  <si>
+    <t>14717652</t>
+  </si>
+  <si>
+    <t>191315</t>
+  </si>
+  <si>
+    <t>116646</t>
+  </si>
+  <si>
+    <t>112571</t>
+  </si>
+  <si>
+    <t>311604</t>
+  </si>
+  <si>
+    <t>114467</t>
+  </si>
+  <si>
+    <t>180580</t>
+  </si>
+  <si>
+    <t>342996</t>
+  </si>
+  <si>
+    <t>136114</t>
+  </si>
+  <si>
+    <t>115469</t>
+  </si>
+  <si>
+    <t>217290</t>
+  </si>
+  <si>
+    <t>116681</t>
+  </si>
+  <si>
+    <t>20374642</t>
+  </si>
+  <si>
+    <t>115476</t>
+  </si>
+  <si>
+    <t>101254</t>
+  </si>
+  <si>
+    <t>946420</t>
+  </si>
+  <si>
+    <t>115785</t>
+  </si>
+  <si>
+    <t>115675</t>
+  </si>
+  <si>
+    <t>815561</t>
+  </si>
+  <si>
+    <t>115746</t>
+  </si>
+  <si>
+    <t>7262858</t>
+  </si>
+  <si>
+    <t>115510</t>
+  </si>
+  <si>
+    <t>182074</t>
+  </si>
+  <si>
+    <t>101491</t>
+  </si>
+  <si>
+    <t>330457</t>
+  </si>
+  <si>
+    <t>OC_UBSLUX</t>
+  </si>
+  <si>
+    <t>101533</t>
+  </si>
+  <si>
+    <t>180992</t>
+  </si>
+  <si>
+    <t>957012</t>
+  </si>
+  <si>
+    <t>25364689</t>
+  </si>
+  <si>
+    <t>218834</t>
+  </si>
+  <si>
+    <t>101605</t>
+  </si>
+  <si>
+    <t>118706</t>
+  </si>
+  <si>
+    <t>101650</t>
+  </si>
+  <si>
+    <t>7698800</t>
+  </si>
+  <si>
+    <t>961642</t>
+  </si>
+  <si>
+    <t>OC_106670</t>
   </si>
 </sst>
 </file>
@@ -379,35 +652,35 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:A16"/>
+  <dimension ref="A1:A98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
@@ -417,57 +690,467 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>2</v>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>